<commit_message>
Still working on the trafo model.
</commit_message>
<xml_diff>
--- a/simplepower/models/grid_data4.xlsx
+++ b/simplepower/models/grid_data4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uisn-my.sharepoint.com/personal/emelf_usn_no/Documents/PhD - SysOpt/Python Work/Custom Modules/simplepower/simplepower/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95E4014C-145F-4665-8D60-87D4A7FA9A82}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{847745D0-9011-4AFC-82C0-BC570AF43379}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>name</t>
   </si>
@@ -81,61 +81,82 @@
     <t>q_nom_mvar</t>
   </si>
   <si>
+    <t>v_nom_pu</t>
+  </si>
+  <si>
+    <t>p_set_mw</t>
+  </si>
+  <si>
+    <t>v_set_pu</t>
+  </si>
+  <si>
+    <t>is_slack</t>
+  </si>
+  <si>
+    <t>S_rated_mva</t>
+  </si>
+  <si>
+    <t>slack</t>
+  </si>
+  <si>
+    <t>S_nom</t>
+  </si>
+  <si>
+    <t>V_hv_kV</t>
+  </si>
+  <si>
+    <t>V_lv_kV</t>
+  </si>
+  <si>
+    <t>V_SCH_pu</t>
+  </si>
+  <si>
+    <t>P_Cu_pu</t>
+  </si>
+  <si>
+    <t>I_E_pu</t>
+  </si>
+  <si>
+    <t>P_Fe_pu</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>idx_hv</t>
+  </si>
+  <si>
+    <t>idx_lv</t>
+  </si>
+  <si>
+    <t>is_pu</t>
+  </si>
+  <si>
+    <t>tap_pos</t>
+  </si>
+  <si>
+    <t>tap_change</t>
+  </si>
+  <si>
+    <t>tap_min</t>
+  </si>
+  <si>
+    <t>tap_max</t>
+  </si>
+  <si>
+    <t>Bus3</t>
+  </si>
+  <si>
+    <t>Line1</t>
+  </si>
+  <si>
     <t>Load 1</t>
   </si>
   <si>
-    <t>v_nom_pu</t>
-  </si>
-  <si>
-    <t>p_set_mw</t>
-  </si>
-  <si>
-    <t>v_set_pu</t>
-  </si>
-  <si>
-    <t>is_slack</t>
-  </si>
-  <si>
-    <t>S_rated_mva</t>
-  </si>
-  <si>
-    <t>slack</t>
-  </si>
-  <si>
-    <t>S_nom</t>
-  </si>
-  <si>
-    <t>V_hv_kV</t>
-  </si>
-  <si>
-    <t>V_lv_kV</t>
-  </si>
-  <si>
-    <t>V_SCH_pu</t>
-  </si>
-  <si>
-    <t>P_Cu_pu</t>
-  </si>
-  <si>
-    <t>I_E_pu</t>
-  </si>
-  <si>
-    <t>P_Fe_pu</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>idx_hv</t>
-  </si>
-  <si>
-    <t>idx_lv</t>
-  </si>
-  <si>
-    <t>is_pu</t>
+    <t>1.0</t>
   </si>
 </sst>
 </file>
@@ -493,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3966F5-6D5F-4BEE-B178-3351115A4B09}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +560,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -546,10 +578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F24F74-C913-4254-AF10-9102B3F26C94}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +619,36 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +661,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -627,19 +688,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
         <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -665,24 +726,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -699,7 +760,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -727,10 +788,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92C15A9-E0D3-48E6-90F6-6A9120B37C7B}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,41 +800,53 @@
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -785,7 +858,7 @@
         <v>22</v>
       </c>
       <c r="E2">
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
       <c r="F2">
         <v>5.0000000000000001E-3</v>
@@ -794,13 +867,25 @@
         <v>0.05</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
         <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0.01</v>
+      </c>
+      <c r="M2">
+        <v>-5</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>